<commit_message>
Update Datasets and KNN
</commit_message>
<xml_diff>
--- a/Paperworks/BPM_Prediction.xlsx
+++ b/Paperworks/BPM_Prediction.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samdy\PycharmProjects\ACR_Test\Paperworks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samdy\PycharmProjects\Bocchi_the_Chord\Paperworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F8414AF-45ED-4D8C-B2B9-616AAB04BA74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D4D6EE0-A0AD-49A2-8479-D07B34A7705C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10560" yWindow="4850" windowWidth="18470" windowHeight="16860" xr2:uid="{0FA0AEE8-F4E0-4FC8-A8BB-1A47062F5A40}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="28800" windowHeight="15830" xr2:uid="{0FA0AEE8-F4E0-4FC8-A8BB-1A47062F5A40}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,18 +56,12 @@
     <t>告白-王欣宇</t>
   </si>
   <si>
-    <t>Precious</t>
-  </si>
-  <si>
     <t>I Really Want to Stay At Your House-Rosa Walton</t>
   </si>
   <si>
     <t>星座になれたら-結束バンド</t>
   </si>
   <si>
-    <t>Genere</t>
-  </si>
-  <si>
     <t>Soundtrack</t>
   </si>
   <si>
@@ -129,6 +123,12 @@
   </si>
   <si>
     <t>红昭愿 - 音阙诗听</t>
+  </si>
+  <si>
+    <t>Precise</t>
+  </si>
+  <si>
+    <t>Genre</t>
   </si>
 </sst>
 </file>
@@ -150,18 +150,24 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Microsoft YaHei UI"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -173,15 +179,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -497,7 +505,7 @@
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -526,36 +534,36 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="G1" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="H1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C2">
-        <v>68</v>
+        <v>123</v>
       </c>
       <c r="D2">
-        <v>68</v>
+        <v>123</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2" t="b">
+      <c r="F2" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="16.5" x14ac:dyDescent="0.4">
@@ -563,7 +571,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>125</v>
@@ -574,11 +582,11 @@
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3" t="b">
+      <c r="F3" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="16.5" x14ac:dyDescent="0.4">
@@ -586,30 +594,30 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C4">
-        <v>123</v>
+        <v>68</v>
       </c>
       <c r="D4">
-        <v>123</v>
+        <v>68</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4" t="b">
+      <c r="F4" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>12</v>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C5">
         <v>70</v>
@@ -620,19 +628,19 @@
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="F5" t="b">
+      <c r="F5" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>14</v>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C6">
         <v>96</v>
@@ -643,19 +651,19 @@
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6" t="b">
+      <c r="F6" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>15</v>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C7">
         <v>180</v>
@@ -666,19 +674,19 @@
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="F7" t="b">
+      <c r="F7" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>16</v>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C8">
         <v>112</v>
@@ -689,19 +697,19 @@
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8" t="b">
+      <c r="F8" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
-        <v>17</v>
+      <c r="B9" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C9">
         <v>172</v>
@@ -712,19 +720,19 @@
       <c r="E9">
         <v>0</v>
       </c>
-      <c r="F9" t="b">
+      <c r="F9" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
-        <v>18</v>
+      <c r="B10" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C10">
         <v>96</v>
@@ -735,19 +743,19 @@
       <c r="E10">
         <v>0</v>
       </c>
-      <c r="F10" t="b">
+      <c r="F10" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
-        <v>19</v>
+      <c r="B11" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C11">
         <v>92</v>
@@ -758,11 +766,11 @@
       <c r="E11">
         <v>0</v>
       </c>
-      <c r="F11" t="b">
+      <c r="F11" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="16.5" x14ac:dyDescent="0.4">
@@ -770,7 +778,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C12">
         <v>120</v>
@@ -781,19 +789,19 @@
       <c r="E12">
         <v>0</v>
       </c>
-      <c r="F12" t="b">
+      <c r="F12" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
-        <v>24</v>
+      <c r="B13" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C13">
         <v>106</v>
@@ -804,19 +812,19 @@
       <c r="E13">
         <v>0</v>
       </c>
-      <c r="F13" t="b">
+      <c r="F13" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
-        <v>26</v>
+      <c r="B14" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C14">
         <v>130</v>
@@ -827,19 +835,19 @@
       <c r="E14">
         <v>0</v>
       </c>
-      <c r="F14" t="b">
+      <c r="F14" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
-        <v>27</v>
+      <c r="B15" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="C15">
         <v>130</v>
@@ -850,19 +858,19 @@
       <c r="E15">
         <v>0</v>
       </c>
-      <c r="F15" t="b">
+      <c r="F15" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
-        <v>28</v>
+      <c r="B16" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C16">
         <v>127</v>
@@ -873,22 +881,22 @@
       <c r="E16">
         <v>0</v>
       </c>
-      <c r="F16" t="b">
+      <c r="F16" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
-        <v>30</v>
+      <c r="B17" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="C17">
         <v>115</v>
@@ -899,11 +907,11 @@
       <c r="E17">
         <v>0</v>
       </c>
-      <c r="F17" t="b">
+      <c r="F17" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
reformat code and add some test data
</commit_message>
<xml_diff>
--- a/Paperworks/BPM_Prediction.xlsx
+++ b/Paperworks/BPM_Prediction.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26519"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samdy\PycharmProjects\Bocchi_the_Chord\Paperworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D4D6EE0-A0AD-49A2-8479-D07B34A7705C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF6FC7C5-7A22-42F3-B1D5-E6077E2A183F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="28800" windowHeight="15830" xr2:uid="{0FA0AEE8-F4E0-4FC8-A8BB-1A47062F5A40}"/>
+    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="21690" xr2:uid="{0FA0AEE8-F4E0-4FC8-A8BB-1A47062F5A40}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -505,7 +505,7 @@
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>